<commit_message>
probando cambios de usuario
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Plan_calidad.xlsx
+++ b/Organización/Calidad/Plan_calidad.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp EliteBook\Documents\Repositorio\SOSQTP\Organización\Calidad\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -119,6 +124,9 @@
   </si>
   <si>
     <t>5 días habiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -628,7 +636,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -639,7 +647,7 @@
   <dimension ref="B3:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -767,6 +775,11 @@
       </c>
       <c r="E12" s="3"/>
     </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Actualizacion plan de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Plan_calidad.xlsx
+++ b/Organización/Calidad/Plan_calidad.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp EliteBook\Documents\Repositorio\SOSQTP\Organización\Calidad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -112,9 +107,6 @@
   </si>
   <si>
     <t>Semestral</t>
-  </si>
-  <si>
-    <t>Requerimientos</t>
   </si>
   <si>
     <t>Estimación</t>
@@ -636,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -646,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -777,7 +769,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -801,20 +793,14 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>26</v>
@@ -879,7 +865,7 @@
         <v>9</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>23</v>
@@ -896,7 +882,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Actualizacon plan de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Plan_calidad.xlsx
+++ b/Organización/Calidad/Plan_calidad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>Plan de proyecto</t>
+  </si>
+  <si>
+    <t>Ticket de servicio</t>
+  </si>
+  <si>
+    <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>Auditoria física y funcional</t>
+  </si>
+  <si>
+    <t>Física</t>
+  </si>
+  <si>
+    <t>Funcional</t>
   </si>
   <si>
     <t>Estrategia de seguimiento</t>
@@ -172,14 +187,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFBDD7EE"/>
+        <bgColor rgb="FFD0CECE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FFD0CECE"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
@@ -247,15 +262,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,11 +278,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,7 +290,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,338 +387,327 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:F65536"/>
+  <dimension ref="B3:F33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.4962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.3740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="32.6259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-    </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="0"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="0"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="0"/>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="0"/>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="0"/>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="0"/>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="0"/>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="0"/>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="0"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="0"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="0"/>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="0"/>
+      <c r="D20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="0"/>
-      <c r="F23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4" t="s">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10" t="s">
+      <c r="C22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="10" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="11" t="s">
+      <c r="C32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C33" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B30:F30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Actualizacion plan de calidad tiempos de ejecucion
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Plan_calidad.xlsx
+++ b/Organización/Calidad/Plan_calidad.xlsx
@@ -138,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -171,6 +171,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -257,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,6 +303,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,7 +402,7 @@
   <dimension ref="B3:F33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -623,7 +635,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>7</v>
@@ -634,13 +646,15 @@
         <v>28</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="10"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
         <v>29</v>
@@ -651,7 +665,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -660,44 +674,44 @@
       <c r="D31" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="12" t="s">
+      <c r="F32" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="12" t="s">
+      <c r="F33" s="13" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificaciones en plan de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Plan_calidad.xlsx
+++ b/Organización/Calidad/Plan_calidad.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -89,10 +89,25 @@
     <t>Plan de proyecto</t>
   </si>
   <si>
+    <t>Adriana Jaramillo</t>
+  </si>
+  <si>
     <t>Ticket de servicio</t>
   </si>
   <si>
     <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>Quincenal</t>
+  </si>
+  <si>
+    <t>Plan de métricas</t>
+  </si>
+  <si>
+    <t>Anuales</t>
+  </si>
+  <si>
+    <t>Plan de Configuración</t>
   </si>
   <si>
     <t>Auditoria física y funcional</t>
@@ -399,10 +414,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:F33"/>
+  <dimension ref="B3:F36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -586,13 +601,13 @@
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>14</v>
@@ -604,115 +619,139 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="8"/>
     </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4"/>
-      <c r="C26" s="4" t="s">
+      <c r="B25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="7" t="s">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="11" t="s">
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="12" t="s">
+      <c r="E34" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="12" t="s">
+      <c r="C35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>36</v>
+      <c r="C36" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -720,8 +759,8 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B33:F33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>